<commit_message>
fixed wrong url redirect issue
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zach\Desktop\projects\ratemydorm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F77C0AE-AB89-43CD-ACF6-EB3351C6408C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47C6004-64BE-4180-9641-D5A633AFD244}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{08953EE4-F8D3-4A45-8A8A-122E90260C4E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="180">
   <si>
     <t>Stanford University</t>
   </si>
@@ -559,6 +559,12 @@
   </si>
   <si>
     <t>UVM</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Nicknames</t>
   </si>
 </sst>
 </file>
@@ -910,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A00701-9303-4C5E-8143-F09AA2C1B703}">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -924,860 +930,766 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>178</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" t="s">
-        <v>102</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>105</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>105</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>116</v>
-      </c>
-      <c r="B14" t="s">
-        <v>94</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>117</v>
       </c>
       <c r="B16" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" t="s">
-        <v>140</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>98</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>141</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" t="s">
-        <v>134</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="B32" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" t="s">
-        <v>143</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="B43" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" t="s">
-        <v>149</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>45</v>
       </c>
       <c r="B52" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>46</v>
+        <v>154</v>
+      </c>
+      <c r="B53" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>47</v>
-      </c>
-      <c r="B54" t="s">
-        <v>127</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B55" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B56" t="s">
-        <v>155</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B57" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B58" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B60" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="B61" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>55</v>
-      </c>
-      <c r="B62" t="s">
-        <v>158</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B63" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B64" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B65" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B66" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B67" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="B68" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>61</v>
+        <v>165</v>
       </c>
       <c r="B69" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="B70" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>63</v>
-      </c>
-      <c r="B71" t="s">
-        <v>167</v>
+        <v>62</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B72" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B73" t="s">
-        <v>129</v>
+        <v>168</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B74" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B75" t="s">
-        <v>130</v>
+        <v>169</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B76" t="s">
-        <v>170</v>
+        <v>130</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B77" t="s">
-        <v>120</v>
+        <v>170</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B78" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B79" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B80" t="s">
-        <v>131</v>
+        <v>171</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B81" t="s">
-        <v>172</v>
+        <v>131</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="B82" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>75</v>
-      </c>
-      <c r="B83" t="s">
-        <v>173</v>
+        <v>74</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B84" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B85" t="s">
-        <v>132</v>
+        <v>174</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="B86" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>79</v>
-      </c>
-      <c r="B87" t="s">
-        <v>133</v>
+        <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B88" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B89" t="s">
-        <v>175</v>
+        <v>134</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="B90" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>83</v>
-      </c>
-      <c r="B91" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B92" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B93" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B94" t="s">
-        <v>176</v>
+        <v>137</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B95" t="s">
-        <v>107</v>
+        <v>176</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B96" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B97" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B98" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="B99" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>92</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
         <v>177</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://www.topuniversities.com/universities/massachusetts-institute-technology-mit" xr:uid="{6BCAF927-A80B-4757-95C4-BEA6DD6CDF07}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://www.topuniversities.com/universities/stanford-university" xr:uid="{D6C962C8-224E-4DA4-9AEE-273BFE56E5C1}"/>
-    <hyperlink ref="A3" r:id="rId3" display="https://www.topuniversities.com/universities/harvard-university" xr:uid="{7C6071B6-0074-4CA4-AEE3-61C47E164D60}"/>
-    <hyperlink ref="A4" r:id="rId4" display="https://www.topuniversities.com/universities/california-institute-technology-caltech" xr:uid="{BF753248-6A92-48AD-A20C-E8AE5E5C6047}"/>
-    <hyperlink ref="A5" r:id="rId5" display="https://www.topuniversities.com/universities/university-chicago" xr:uid="{51D82205-3FEF-40C8-BE9F-BCC4FC169089}"/>
-    <hyperlink ref="A6" r:id="rId6" display="https://www.topuniversities.com/universities/princeton-university" xr:uid="{94550525-3F76-4C99-96E1-86C0AF9A026C}"/>
-    <hyperlink ref="A7" r:id="rId7" display="https://www.topuniversities.com/universities/cornell-university" xr:uid="{1BD6C41C-25CC-4FBD-94E3-896E1B6314CA}"/>
-    <hyperlink ref="A8" r:id="rId8" display="https://www.topuniversities.com/universities/yale-university" xr:uid="{F9278C1D-69E3-47E1-A94D-212ECE79DC71}"/>
-    <hyperlink ref="A9" r:id="rId9" display="https://www.topuniversities.com/universities/columbia-university" xr:uid="{C9488393-00AA-4A58-A3A1-72242530A7E2}"/>
-    <hyperlink ref="A10" r:id="rId10" display="https://www.topuniversities.com/universities/university-pennsylvania" xr:uid="{B8F92A79-48DC-4A1C-87D2-8F07388580C7}"/>
-    <hyperlink ref="A11" r:id="rId11" display="https://www.topuniversities.com/universities/university-michigan" xr:uid="{476BAFE3-E5DA-43FA-AA73-B7A701FA1843}"/>
-    <hyperlink ref="A12" r:id="rId12" display="https://www.topuniversities.com/universities/johns-hopkins-university" xr:uid="{CA957416-65C1-4EF8-B94D-3B142A587117}"/>
-    <hyperlink ref="A13" r:id="rId13" display="https://www.topuniversities.com/universities/duke-university" xr:uid="{6BCA2B8A-0253-475F-97B4-2C68B524536A}"/>
-    <hyperlink ref="A14" r:id="rId14" display="https://www.topuniversities.com/universities/university-california-berkeley-ucb" xr:uid="{899D01A5-F419-4508-A477-F63A7210A07E}"/>
-    <hyperlink ref="A15" r:id="rId15" display="https://www.topuniversities.com/universities/university-california-los-angeles-ucla" xr:uid="{C55412FF-6C30-4FE3-BB5D-AA1984FF1816}"/>
-    <hyperlink ref="A16" r:id="rId16" display="https://www.topuniversities.com/universities/northwestern-university" xr:uid="{D1F65166-643C-4C86-8CB6-40458F5B40DA}"/>
-    <hyperlink ref="A17" r:id="rId17" display="https://www.topuniversities.com/universities/university-california-san-diego-ucsd" xr:uid="{AB88B681-3BE6-4954-8ACB-C293919736C4}"/>
-    <hyperlink ref="A18" r:id="rId18" display="https://www.topuniversities.com/universities/new-york-university-nyu" xr:uid="{58BE94FE-5E71-430C-8C04-71993DCA5D78}"/>
-    <hyperlink ref="A19" r:id="rId19" display="https://www.topuniversities.com/universities/carnegie-mellon-university" xr:uid="{D5B78CD6-93BF-4F36-8687-4790E8EA4ED9}"/>
-    <hyperlink ref="A20" r:id="rId20" display="https://www.topuniversities.com/universities/university-wisconsin-madison" xr:uid="{1556794A-E22E-47AA-9876-965212FB1F03}"/>
-    <hyperlink ref="A21" r:id="rId21" display="https://www.topuniversities.com/universities/brown-university" xr:uid="{778122DA-0FF5-4C53-A712-22179BE3BA7B}"/>
-    <hyperlink ref="A22" r:id="rId22" display="https://www.topuniversities.com/universities/university-texas-austin" xr:uid="{434E610E-105B-47F4-87CF-09085EF26BC0}"/>
-    <hyperlink ref="A23" r:id="rId23" display="https://www.topuniversities.com/universities/university-washington" xr:uid="{CFDF068F-889F-4E32-8DF2-B8E24F4DE352}"/>
-    <hyperlink ref="A24" r:id="rId24" display="https://www.topuniversities.com/universities/georgia-institute-technology" xr:uid="{5F181020-82CC-4E88-8B5B-F26E0E4C25D1}"/>
-    <hyperlink ref="A25" r:id="rId25" display="https://www.topuniversities.com/universities/university-illinois-urbana-champaign" xr:uid="{03A62846-287C-4BBD-9516-E75307F56A13}"/>
-    <hyperlink ref="A26" r:id="rId26" display="https://www.topuniversities.com/universities/university-north-carolina-chapel-hill" xr:uid="{FFA99382-AE6F-41DE-B797-5FB76B274788}"/>
-    <hyperlink ref="A27" r:id="rId27" display="https://www.topuniversities.com/universities/rice-university" xr:uid="{0D92F9EB-F4AC-41DD-B45F-10AC6EC8912C}"/>
-    <hyperlink ref="A28" r:id="rId28" display="https://www.topuniversities.com/universities/ohio-state-university" xr:uid="{38E7251C-AB56-4F9B-8F40-5889B161B958}"/>
-    <hyperlink ref="A29" r:id="rId29" display="https://www.topuniversities.com/universities/boston-university" xr:uid="{E2BF2E4F-56AF-4EE3-86B8-74B7139889CD}"/>
-    <hyperlink ref="A30" r:id="rId30" display="https://www.topuniversities.com/universities/pennsylvania-state-university" xr:uid="{2C0BD9DF-4D85-442D-8931-A1930C47BFCC}"/>
-    <hyperlink ref="A31" r:id="rId31" display="https://www.topuniversities.com/universities/washington-university-st-louis" xr:uid="{7C13747C-C2EF-466D-BCC1-AE7E7D17513F}"/>
-    <hyperlink ref="A32" r:id="rId32" display="https://www.topuniversities.com/universities/purdue-university" xr:uid="{1C7E0675-5124-44AE-80BD-6458F1F3C046}"/>
-    <hyperlink ref="A33" r:id="rId33" display="https://www.topuniversities.com/universities/university-california-davis" xr:uid="{6053A1F8-70E6-4AA5-A33E-437AF68F289F}"/>
-    <hyperlink ref="A34" r:id="rId34" display="https://www.topuniversities.com/universities/university-southern-california" xr:uid="{1D7BBA47-798E-464F-9542-608E266185AD}"/>
-    <hyperlink ref="A35" r:id="rId35" display="https://www.topuniversities.com/universities/university-maryland-college-park" xr:uid="{EE3891B4-EC2D-45EE-B376-366E25FCDFFB}"/>
-    <hyperlink ref="A36" r:id="rId36" display="https://www.topuniversities.com/universities/university-california-santa-barbara-ucsb" xr:uid="{C79BA399-2483-453F-B50F-94CD62003079}"/>
-    <hyperlink ref="A37" r:id="rId37" display="https://www.topuniversities.com/universities/university-pittsburgh" xr:uid="{754279DB-229F-41CB-BDAB-8108B05EBC30}"/>
-    <hyperlink ref="A38" r:id="rId38" display="https://www.topuniversities.com/universities/michigan-state-university" xr:uid="{A7EB080D-3C45-4C20-AF98-D456ACEF15E1}"/>
-    <hyperlink ref="A39" r:id="rId39" display="https://www.topuniversities.com/universities/emory-university" xr:uid="{093C6E42-FE55-4D1A-A7A9-82064FDC2BAE}"/>
-    <hyperlink ref="A40" r:id="rId40" display="https://www.topuniversities.com/universities/university-minnesota" xr:uid="{5E8A136F-AC18-49BD-9387-74938EE3F4DE}"/>
-    <hyperlink ref="A41" r:id="rId41" display="https://www.topuniversities.com/universities/university-california-irvine" xr:uid="{4BFEFB1F-E73A-42BE-90B5-2A8D2774FF36}"/>
-    <hyperlink ref="A42" r:id="rId42" display="https://www.topuniversities.com/universities/university-florida" xr:uid="{C9EF0E5C-F675-4FFB-99C9-22D823C436F6}"/>
-    <hyperlink ref="A43" r:id="rId43" display="https://www.topuniversities.com/universities/dartmouth-college" xr:uid="{38F126FA-20F5-4136-B994-2A274C84543B}"/>
-    <hyperlink ref="A44" r:id="rId44" display="https://www.topuniversities.com/universities/university-rochester" xr:uid="{E27D6B1C-CAA7-4F39-98D9-AA1E7F063CCE}"/>
-    <hyperlink ref="A45" r:id="rId45" display="https://www.topuniversities.com/universities/case-western-reserve-university" xr:uid="{1F9EB3FD-37BB-4771-9506-3C9CF88D2E1E}"/>
-    <hyperlink ref="A46" r:id="rId46" display="https://www.topuniversities.com/universities/university-colorado-boulder" xr:uid="{C472B0E4-1CA1-4D5A-8833-3FD9F4294C22}"/>
-    <hyperlink ref="A47" r:id="rId47" display="https://www.topuniversities.com/universities/university-virginia" xr:uid="{CF380BB4-B0A8-401F-AF93-80D8E81C0ABE}"/>
-    <hyperlink ref="A48" r:id="rId48" display="https://www.topuniversities.com/universities/vanderbilt-university" xr:uid="{0357F3EC-D4D6-45A1-B367-38DF6076C3EC}"/>
-    <hyperlink ref="A49" r:id="rId49" display="https://www.topuniversities.com/universities/texas-am-university" xr:uid="{6E79E4A0-12AD-4B18-A7F4-E6A9FC566248}"/>
-    <hyperlink ref="A50" r:id="rId50" display="https://www.topuniversities.com/universities/arizona-state-university" xr:uid="{C1B6F14C-A668-4EFF-ACC0-A127F1352D18}"/>
-    <hyperlink ref="A51" r:id="rId51" display="https://www.topuniversities.com/universities/university-notre-dame" xr:uid="{384C3DD6-F8C1-4849-9070-5D9FA010AF20}"/>
-    <hyperlink ref="A52" r:id="rId52" display="https://www.topuniversities.com/universities/university-illinois-chicago-uic" xr:uid="{6C967EAA-D70D-43C7-A95A-1BF47C1BD300}"/>
-    <hyperlink ref="A53" r:id="rId53" display="https://www.topuniversities.com/universities/georgetown-university" xr:uid="{5249E8ED-C746-4C31-B26C-8FCCB5B37FB3}"/>
-    <hyperlink ref="A54" r:id="rId54" display="https://www.topuniversities.com/universities/tufts-university" xr:uid="{CAEC54D3-EFDA-4F3F-80A4-13770E128290}"/>
-    <hyperlink ref="A55" r:id="rId55" display="https://www.topuniversities.com/universities/university-miami" xr:uid="{1E861112-2EA3-4128-8067-4B167E070F70}"/>
-    <hyperlink ref="A56" r:id="rId56" display="https://www.topuniversities.com/universities/university-arizona" xr:uid="{F14873F5-98DB-4419-B605-97DF7791E0B7}"/>
-    <hyperlink ref="A57" r:id="rId57" display="https://www.topuniversities.com/universities/university-massachusetts-amherst" xr:uid="{1CA0262E-919A-41C0-B73B-F7F0E248A19B}"/>
-    <hyperlink ref="A58" r:id="rId58" display="https://www.topuniversities.com/universities/north-carolina-state-university" xr:uid="{052DD493-F1D3-4520-B9D0-A7F7D8F702A1}"/>
-    <hyperlink ref="A59" r:id="rId59" display="https://www.topuniversities.com/universities/rutgers-university-new-brunswick" xr:uid="{5A41014F-F7C0-4C3A-9205-B8524E528B4B}"/>
-    <hyperlink ref="A60" r:id="rId60" display="https://www.topuniversities.com/universities/university-hawaii-ma%C3%B1oa" xr:uid="{1248899F-2437-4083-8BB9-3EB12D892986}"/>
-    <hyperlink ref="A61" r:id="rId61" display="https://www.topuniversities.com/universities/yeshiva-university" xr:uid="{5B5A345A-2411-4DBA-8849-CF1FCDF6A4B0}"/>
-    <hyperlink ref="A62" r:id="rId62" display="https://www.topuniversities.com/universities/university-buffalo-suny" xr:uid="{B70C4946-D7CA-4DA2-BA7A-C822574CAAEB}"/>
-    <hyperlink ref="A63" r:id="rId63" display="https://www.topuniversities.com/universities/indiana-university-bloomington" xr:uid="{66C0FB89-90DC-4E83-BAB8-5C71C2983BBF}"/>
-    <hyperlink ref="A64" r:id="rId64" display="https://www.topuniversities.com/universities/northeastern-university" xr:uid="{6175510F-7655-4E50-AD5A-9805B99ED5E1}"/>
-    <hyperlink ref="A65" r:id="rId65" display="https://www.topuniversities.com/universities/university-california-santa-cruz" xr:uid="{196FBA9A-F90B-4084-9DEC-12DD51D3059E}"/>
-    <hyperlink ref="A66" r:id="rId66" display="https://www.topuniversities.com/universities/virginia-polytechnic-institute-virginia-tech" xr:uid="{E3BCB49A-85A0-416A-9A1F-0B89D2CD1FA0}"/>
-    <hyperlink ref="A67" r:id="rId67" display="https://www.topuniversities.com/universities/george-washington-university" xr:uid="{5D0CC842-3168-45AB-B8A2-FCBB6959CC53}"/>
-    <hyperlink ref="A68" r:id="rId68" display="https://www.topuniversities.com/universities/rensselaer-polytechnic-institute" xr:uid="{61404F61-0C84-46BF-A1D1-CC72C4E3D429}"/>
-    <hyperlink ref="A69" r:id="rId69" display="https://www.topuniversities.com/universities/university-utah" xr:uid="{749C3838-57DF-4EDD-A082-A48A407D969D}"/>
-    <hyperlink ref="A70" r:id="rId70" display="https://www.topuniversities.com/universities/stony-brook-university-state-university-new-york" xr:uid="{6D3B013A-DBC1-4913-8A45-F8E4C7115CF9}"/>
-    <hyperlink ref="A71" r:id="rId71" display="https://www.topuniversities.com/universities/university-kansas" xr:uid="{18A799F4-FB24-40D6-B1CE-1630E9713571}"/>
-    <hyperlink ref="A72" r:id="rId72" display="https://www.topuniversities.com/universities/university-connecticut" xr:uid="{15C5A627-00F8-4CE2-9314-F7C15207E8A8}"/>
-    <hyperlink ref="A73" r:id="rId73" display="https://www.topuniversities.com/universities/boston-college" xr:uid="{08160E0F-6B6B-4EE8-9F95-158A8A1DAB13}"/>
-    <hyperlink ref="A74" r:id="rId74" display="https://www.topuniversities.com/universities/university-california-riverside" xr:uid="{D9A2DFB7-909B-4724-9B7D-5C01CC623FD3}"/>
-    <hyperlink ref="A75" r:id="rId75" display="https://www.topuniversities.com/universities/wake-forest-university" xr:uid="{B05DA855-8F06-4D07-B8AE-9792CD64BC6E}"/>
-    <hyperlink ref="A76" r:id="rId76" display="https://www.topuniversities.com/universities/washington-state-university" xr:uid="{57E01D8D-3D35-4E4B-88E8-C2B61EF49319}"/>
-    <hyperlink ref="A77" r:id="rId77" display="https://www.topuniversities.com/universities/university-colorado-denver" xr:uid="{5FE63D32-5329-436D-8E00-61B41CAB077F}"/>
-    <hyperlink ref="A78" r:id="rId78" display="https://www.topuniversities.com/universities/tulane-university" xr:uid="{3B91B089-2CD0-4347-B2C0-1DEB57E9487D}"/>
-    <hyperlink ref="A79" r:id="rId79" display="https://www.topuniversities.com/universities/university-tennessee-knoxville" xr:uid="{2ECF70FA-F857-454C-BB7C-607823F0740F}"/>
-    <hyperlink ref="A80" r:id="rId80" display="https://www.topuniversities.com/universities/illinois-institute-technology" xr:uid="{26984486-EB0F-43F7-992C-B65180209CFD}"/>
-    <hyperlink ref="A81" r:id="rId81" display="https://www.topuniversities.com/universities/university-texas-dallas" xr:uid="{3C89CEB1-7A9F-489C-B3D9-F2C678DFC929}"/>
-    <hyperlink ref="A82" r:id="rId82" display="https://www.topuniversities.com/universities/brandeis-university" xr:uid="{667BA57C-501A-45DA-B99D-2DB8E55EC22E}"/>
-    <hyperlink ref="A83" r:id="rId83" display="https://www.topuniversities.com/universities/university-georgia" xr:uid="{2FCB9A1C-4F46-4E4E-8A7E-9231F7228832}"/>
-    <hyperlink ref="A84" r:id="rId84" display="https://www.topuniversities.com/universities/university-iowa" xr:uid="{511893F0-2867-43B8-A627-4410089198F1}"/>
-    <hyperlink ref="A85" r:id="rId85" display="https://www.topuniversities.com/universities/university-delaware" xr:uid="{76E3444E-4EC0-4833-8055-A5F304A22000}"/>
-    <hyperlink ref="A86" r:id="rId86" display="https://www.topuniversities.com/universities/wayne-state-university" xr:uid="{83746B27-57FB-4A7C-9D64-A3E4AF01A160}"/>
-    <hyperlink ref="A87" r:id="rId87" display="https://www.topuniversities.com/universities/colorado-state-university" xr:uid="{679AABB8-2678-41C5-B917-46D617CBB167}"/>
-    <hyperlink ref="A88" r:id="rId88" display="https://www.topuniversities.com/universities/oregon-state-university" xr:uid="{81CB4CA8-F76E-476E-89B1-B6D6B85CBB1E}"/>
-    <hyperlink ref="A89" r:id="rId89" display="https://www.topuniversities.com/universities/university-maryland-baltimore-county" xr:uid="{6A7D3835-764C-482D-8AB9-832B6DE9569F}"/>
-    <hyperlink ref="A90" r:id="rId90" display="https://www.topuniversities.com/universities/clark-university" xr:uid="{CDC02644-91B5-4F24-A65C-4186D1804E17}"/>
-    <hyperlink ref="A91" r:id="rId91" display="https://www.topuniversities.com/universities/florida-state-university" xr:uid="{90B79031-E425-494E-977A-328A87CD3250}"/>
-    <hyperlink ref="A92" r:id="rId92" display="https://www.topuniversities.com/universities/iowa-state-university" xr:uid="{B01EAB5F-1070-44EF-8D02-0A42E24B820A}"/>
-    <hyperlink ref="A93" r:id="rId93" display="https://www.topuniversities.com/universities/university-new-mexico" xr:uid="{C6F921DE-4882-45DF-B152-B0F5025E201A}"/>
-    <hyperlink ref="A94" r:id="rId94" display="https://www.topuniversities.com/universities/university-oklahoma" xr:uid="{A1607B9B-6FF9-4F85-81AD-FA4427D75862}"/>
-    <hyperlink ref="A95" r:id="rId95" display="https://www.topuniversities.com/universities/drexel-university" xr:uid="{CE7B7B0A-C6B4-4D71-B796-511509E9CB64}"/>
-    <hyperlink ref="A96" r:id="rId96" display="https://www.topuniversities.com/universities/lehigh-university" xr:uid="{93E29A63-9D15-4D23-9D62-75C7A4EEBE7F}"/>
-    <hyperlink ref="A97" r:id="rId97" display="https://www.topuniversities.com/universities/howard-university" xr:uid="{528E4858-69E2-489F-A250-7B0F0373D407}"/>
-    <hyperlink ref="A98" r:id="rId98" display="https://www.topuniversities.com/universities/university-south-florida" xr:uid="{70EF4253-1682-42C9-9E56-EB785F618BB5}"/>
-    <hyperlink ref="A99" r:id="rId99" display="https://www.topuniversities.com/universities/new-school" xr:uid="{E8637890-3896-4BFA-A933-4FCA54F9B7FA}"/>
-    <hyperlink ref="A100" r:id="rId100" display="https://www.topuniversities.com/universities/university-vermont" xr:uid="{951DB1E3-0684-47EA-A151-9060B6A073D5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId101"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed dorm page bugs
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zach\Desktop\projects\ratemydorm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47C6004-64BE-4180-9641-D5A633AFD244}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E31E327-4B89-4E36-B358-12B324D4E7DB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{08953EE4-F8D3-4A45-8A8A-122E90260C4E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="242">
   <si>
     <t>Stanford University</t>
   </si>
@@ -565,6 +565,192 @@
   </si>
   <si>
     <t>Nicknames</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Stanford</t>
+  </si>
+  <si>
+    <t>Harvard</t>
+  </si>
+  <si>
+    <t>Princeton</t>
+  </si>
+  <si>
+    <t>Cornell</t>
+  </si>
+  <si>
+    <t>Yale</t>
+  </si>
+  <si>
+    <t>Columbia</t>
+  </si>
+  <si>
+    <t>Duke</t>
+  </si>
+  <si>
+    <t>Northwestern</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>UPenn</t>
+  </si>
+  <si>
+    <t>UWMadison</t>
+  </si>
+  <si>
+    <t>UT-Austin</t>
+  </si>
+  <si>
+    <t>UChicago</t>
+  </si>
+  <si>
+    <t>UC-Berkeley</t>
+  </si>
+  <si>
+    <t>WUSTL</t>
+  </si>
+  <si>
+    <t>Purdue</t>
+  </si>
+  <si>
+    <t>UC-Davis</t>
+  </si>
+  <si>
+    <t>Emory</t>
+  </si>
+  <si>
+    <t>UMN</t>
+  </si>
+  <si>
+    <t>UC-Irvine</t>
+  </si>
+  <si>
+    <t>Dartmouth</t>
+  </si>
+  <si>
+    <t>Rochester</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Vanderbilt</t>
+  </si>
+  <si>
+    <t>Georgetown</t>
+  </si>
+  <si>
+    <t>Tufts</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>UMass</t>
+  </si>
+  <si>
+    <t>Rutgers</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>YU</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
+  </si>
+  <si>
+    <t>IUB</t>
+  </si>
+  <si>
+    <t>Northeastern</t>
+  </si>
+  <si>
+    <t>UCSC</t>
+  </si>
+  <si>
+    <t>VirginiaTech</t>
+  </si>
+  <si>
+    <t>GWU</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>StonyBrook</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>UConn</t>
+  </si>
+  <si>
+    <t>UCR</t>
+  </si>
+  <si>
+    <t>WakeForest</t>
+  </si>
+  <si>
+    <t>WSU</t>
+  </si>
+  <si>
+    <t>Tulane</t>
+  </si>
+  <si>
+    <t>UT-Knoxville</t>
+  </si>
+  <si>
+    <t>UT-Dallas</t>
+  </si>
+  <si>
+    <t>Brandeis</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>Wayne</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>OregonState</t>
+  </si>
+  <si>
+    <t>UMBC</t>
+  </si>
+  <si>
+    <t>Drexel</t>
+  </si>
+  <si>
+    <t>Lehigh</t>
+  </si>
+  <si>
+    <t>Howard</t>
+  </si>
+  <si>
+    <t>NewSchool</t>
+  </si>
+  <si>
+    <t>UDel</t>
   </si>
 </sst>
 </file>
@@ -916,775 +1102,1079 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A00701-9303-4C5E-8143-F09AA2C1B703}">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="50.6640625" customWidth="1"/>
     <col min="2" max="2" width="47.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>178</v>
       </c>
       <c r="B1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>100</v>
       </c>
       <c r="B2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>101</v>
       </c>
       <c r="B5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>116</v>
       </c>
       <c r="B15" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>117</v>
       </c>
       <c r="B16" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>118</v>
       </c>
       <c r="B18" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
       <c r="B19" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>13</v>
       </c>
       <c r="B20" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>14</v>
       </c>
       <c r="B21" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
       <c r="B23" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
       <c r="B24" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>18</v>
       </c>
       <c r="B25" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>19</v>
       </c>
       <c r="B26" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>20</v>
       </c>
       <c r="B27" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>22</v>
       </c>
       <c r="B29" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>23</v>
       </c>
       <c r="B30" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>24</v>
       </c>
       <c r="B31" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>25</v>
       </c>
       <c r="B32" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>27</v>
       </c>
       <c r="B34" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>28</v>
       </c>
       <c r="B35" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>29</v>
       </c>
       <c r="B36" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>30</v>
       </c>
       <c r="B37" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>31</v>
       </c>
       <c r="B38" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>32</v>
       </c>
       <c r="B39" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>34</v>
       </c>
       <c r="B41" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>35</v>
       </c>
       <c r="B42" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>36</v>
       </c>
       <c r="B43" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>38</v>
       </c>
       <c r="B45" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>39</v>
       </c>
       <c r="B46" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>40</v>
       </c>
       <c r="B47" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>41</v>
       </c>
       <c r="B48" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>42</v>
       </c>
       <c r="B49" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>43</v>
       </c>
       <c r="B50" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>44</v>
       </c>
       <c r="B51" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>45</v>
       </c>
       <c r="B52" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>154</v>
       </c>
       <c r="B53" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>47</v>
       </c>
       <c r="B55" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>48</v>
       </c>
       <c r="B56" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>49</v>
       </c>
       <c r="B57" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>50</v>
       </c>
       <c r="B58" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>51</v>
       </c>
       <c r="B59" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>52</v>
       </c>
       <c r="B60" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>53</v>
       </c>
       <c r="B61" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>55</v>
       </c>
       <c r="B63" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>56</v>
       </c>
       <c r="B64" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>57</v>
       </c>
       <c r="B65" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>58</v>
       </c>
       <c r="B66" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>59</v>
       </c>
       <c r="B67" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>60</v>
       </c>
       <c r="B68" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>165</v>
       </c>
       <c r="B69" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>61</v>
       </c>
       <c r="B70" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C71" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>63</v>
       </c>
       <c r="B72" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>64</v>
       </c>
       <c r="B73" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C73" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>65</v>
       </c>
       <c r="B74" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>66</v>
       </c>
       <c r="B75" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C75" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>67</v>
       </c>
       <c r="B76" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C76" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>68</v>
       </c>
       <c r="B77" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C77" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>69</v>
       </c>
       <c r="B78" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>70</v>
       </c>
       <c r="B79" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C79" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>71</v>
       </c>
       <c r="B80" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C80" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>72</v>
       </c>
       <c r="B81" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C81" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>73</v>
       </c>
       <c r="B82" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C82" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C83" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>75</v>
       </c>
       <c r="B84" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C84" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>76</v>
       </c>
       <c r="B85" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C85" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>77</v>
       </c>
       <c r="B86" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C86" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C87" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>79</v>
       </c>
       <c r="B88" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C88" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>80</v>
       </c>
       <c r="B89" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C89" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>81</v>
       </c>
       <c r="B90" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C90" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C91" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>83</v>
       </c>
       <c r="B92" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C92" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>84</v>
       </c>
       <c r="B93" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C93" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>85</v>
       </c>
       <c r="B94" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C94" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>86</v>
       </c>
       <c r="B95" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C95" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>87</v>
       </c>
       <c r="B96" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C96" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>88</v>
       </c>
       <c r="B97" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C97" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>89</v>
       </c>
       <c r="B98" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C98" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>90</v>
       </c>
       <c r="B99" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C99" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C100" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>92</v>
       </c>
       <c r="B101" t="s">
+        <v>177</v>
+      </c>
+      <c r="C101" t="s">
         <v>177</v>
       </c>
     </row>

</xml_diff>